<commit_message>
Update CRONOGRAMA TECNOLOGICO HUANCARAMA.xlsx
</commit_message>
<xml_diff>
--- a/CRONOGRAMA TECNOLOGICO HUANCARAMA.xlsx
+++ b/CRONOGRAMA TECNOLOGICO HUANCARAMA.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22730"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22827"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="J:\PROYECTOS INVIERTE.PE\10. INSTITUTO HUANCARAMA\PLAN DE TRABAJO INSTITUTO\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\RepositorioORFEI\PROYECTO-035-Int-Huancarama\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F1579733-63F6-43D5-9BCB-5375EBB5774E}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E1A00BB8-167A-4C4D-846D-C1BF902FB5AB}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="30936" windowHeight="16896" tabRatio="696" activeTab="1" xr2:uid="{2012C5C9-856F-4F31-AA7F-E5F916677A76}"/>
+    <workbookView xWindow="870" yWindow="8565" windowWidth="13800" windowHeight="9495" tabRatio="696" activeTab="1" xr2:uid="{2012C5C9-856F-4F31-AA7F-E5F916677A76}"/>
   </bookViews>
   <sheets>
     <sheet name="Profesionales" sheetId="2" r:id="rId1"/>
@@ -1460,11 +1460,62 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="2" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="3" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="4" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="6" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="9" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="10" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="10" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="11" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="11" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -1487,39 +1538,6 @@
     <xf numFmtId="0" fontId="10" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="9" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="10" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="10" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="11" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="11" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="2" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="3" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="4" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -1527,24 +1545,6 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="6" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -2126,25 +2126,25 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9570033D-1DAE-4073-9A8B-C82240EAFBC8}">
   <dimension ref="A3:F15"/>
   <sheetViews>
-    <sheetView showGridLines="0" topLeftCell="A7" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+    <sheetView showGridLines="0" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
       <selection activeCell="B17" sqref="B17"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="12" defaultRowHeight="13.8" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="12" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="8.125" style="1" customWidth="1"/>
-    <col min="2" max="2" width="30.375" style="1" customWidth="1"/>
-    <col min="3" max="3" width="39.875" style="1" customWidth="1"/>
+    <col min="1" max="1" width="8.1640625" style="1" customWidth="1"/>
+    <col min="2" max="2" width="30.33203125" style="1" customWidth="1"/>
+    <col min="3" max="3" width="39.83203125" style="1" customWidth="1"/>
     <col min="4" max="4" width="140" style="1" customWidth="1"/>
-    <col min="5" max="5" width="15.625" style="1" customWidth="1"/>
-    <col min="6" max="6" width="16.375" style="1" customWidth="1"/>
+    <col min="5" max="5" width="15.6640625" style="1" customWidth="1"/>
+    <col min="6" max="6" width="16.33203125" style="1" customWidth="1"/>
     <col min="7" max="7" width="12" style="1"/>
-    <col min="8" max="8" width="15.875" style="1" customWidth="1"/>
-    <col min="9" max="9" width="105.875" style="1" customWidth="1"/>
+    <col min="8" max="8" width="15.83203125" style="1" customWidth="1"/>
+    <col min="9" max="9" width="105.83203125" style="1" customWidth="1"/>
     <col min="10" max="16384" width="12" style="1"/>
   </cols>
   <sheetData>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A3" s="92" t="s">
         <v>4</v>
       </c>
@@ -2160,7 +2160,7 @@
       <c r="E3" s="12"/>
       <c r="F3" s="12"/>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A4" s="93"/>
       <c r="B4" s="4" t="s">
         <v>10</v>
@@ -2170,7 +2170,7 @@
       <c r="E4" s="12"/>
       <c r="F4" s="12"/>
     </row>
-    <row r="5" spans="1:6" ht="82.8" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:6" ht="76.5" x14ac:dyDescent="0.2">
       <c r="A5" s="14">
         <v>1</v>
       </c>
@@ -2186,7 +2186,7 @@
       <c r="E5" s="12"/>
       <c r="F5" s="12"/>
     </row>
-    <row r="6" spans="1:6" ht="179.4" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:6" ht="165.75" x14ac:dyDescent="0.2">
       <c r="A6" s="2">
         <v>2</v>
       </c>
@@ -2202,7 +2202,7 @@
       <c r="E6" s="13"/>
       <c r="F6" s="13"/>
     </row>
-    <row r="7" spans="1:6" ht="69" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:6" ht="63.75" x14ac:dyDescent="0.2">
       <c r="A7" s="16">
         <v>4</v>
       </c>
@@ -2218,7 +2218,7 @@
       <c r="E7" s="13"/>
       <c r="F7" s="13"/>
     </row>
-    <row r="8" spans="1:6" ht="179.4" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:6" ht="165.75" x14ac:dyDescent="0.2">
       <c r="A8" s="15">
         <v>5</v>
       </c>
@@ -2234,7 +2234,7 @@
       <c r="E8" s="13"/>
       <c r="F8" s="13"/>
     </row>
-    <row r="9" spans="1:6" ht="69" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:6" ht="63.75" x14ac:dyDescent="0.2">
       <c r="A9" s="16">
         <v>6</v>
       </c>
@@ -2250,7 +2250,7 @@
       <c r="E9" s="13"/>
       <c r="F9" s="13"/>
     </row>
-    <row r="10" spans="1:6" ht="27.6" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:6" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A10" s="16">
         <v>7</v>
       </c>
@@ -2266,7 +2266,7 @@
       <c r="E10" s="13"/>
       <c r="F10" s="13"/>
     </row>
-    <row r="11" spans="1:6" ht="69" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:6" ht="63.75" x14ac:dyDescent="0.2">
       <c r="A11" s="15">
         <v>8</v>
       </c>
@@ -2282,7 +2282,7 @@
       <c r="E11" s="13"/>
       <c r="F11" s="13"/>
     </row>
-    <row r="12" spans="1:6" ht="27.6" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:6" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A12" s="29">
         <v>9</v>
       </c>
@@ -2298,7 +2298,7 @@
       <c r="E12" s="13"/>
       <c r="F12" s="13"/>
     </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A13" s="2"/>
       <c r="B13" s="4" t="s">
         <v>11</v>
@@ -2308,7 +2308,7 @@
       <c r="E13" s="13"/>
       <c r="F13" s="13"/>
     </row>
-    <row r="14" spans="1:6" ht="55.2" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:6" ht="51" x14ac:dyDescent="0.2">
       <c r="A14" s="2">
         <v>1</v>
       </c>
@@ -2324,7 +2324,7 @@
       <c r="E14" s="13"/>
       <c r="F14" s="13"/>
     </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A15" s="1">
         <v>2</v>
       </c>
@@ -2350,68 +2350,73 @@
   <dimension ref="A1:CR102"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <pane xSplit="5" ySplit="4" topLeftCell="AN52" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="5" ySplit="4" topLeftCell="F39" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="F1" sqref="F1"/>
       <selection pane="bottomLeft" activeCell="A5" sqref="A5"/>
-      <selection pane="bottomRight" activeCell="BD68" sqref="BD68"/>
+      <selection pane="bottomRight" activeCell="CU87" sqref="CU87"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="12" defaultRowHeight="10.199999999999999" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="12" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="6.875" style="38" customWidth="1"/>
-    <col min="2" max="2" width="75.375" style="38" customWidth="1"/>
-    <col min="3" max="3" width="20.25" style="65" customWidth="1"/>
+    <col min="1" max="1" width="6.83203125" style="38" customWidth="1"/>
+    <col min="2" max="2" width="75.33203125" style="38" customWidth="1"/>
+    <col min="3" max="3" width="20.1640625" style="65" customWidth="1"/>
     <col min="4" max="5" width="12" style="38"/>
-    <col min="6" max="6" width="6.875" style="38" customWidth="1"/>
+    <col min="6" max="6" width="6.83203125" style="38" customWidth="1"/>
     <col min="7" max="7" width="7" style="38" customWidth="1"/>
     <col min="8" max="8" width="5" style="38" customWidth="1"/>
-    <col min="9" max="11" width="4.375" style="38" customWidth="1"/>
-    <col min="12" max="13" width="3.375" style="38" customWidth="1"/>
+    <col min="9" max="11" width="4.33203125" style="38" customWidth="1"/>
+    <col min="12" max="13" width="3.33203125" style="38" customWidth="1"/>
     <col min="14" max="14" width="3" style="38" customWidth="1"/>
     <col min="15" max="15" width="3.5" style="38" customWidth="1"/>
-    <col min="16" max="16" width="3.375" style="38" customWidth="1"/>
-    <col min="17" max="17" width="3.125" style="38" customWidth="1"/>
-    <col min="18" max="19" width="3.625" style="38" customWidth="1"/>
-    <col min="20" max="20" width="3.125" style="38" customWidth="1"/>
-    <col min="21" max="24" width="3.375" style="38" customWidth="1"/>
-    <col min="25" max="31" width="3" style="38" customWidth="1"/>
-    <col min="32" max="32" width="3.125" style="38" customWidth="1"/>
+    <col min="16" max="16" width="3.33203125" style="38" customWidth="1"/>
+    <col min="17" max="17" width="3.1640625" style="38" customWidth="1"/>
+    <col min="18" max="19" width="3.6640625" style="38" customWidth="1"/>
+    <col min="20" max="20" width="3.1640625" style="38" customWidth="1"/>
+    <col min="21" max="24" width="3.33203125" style="38" customWidth="1"/>
+    <col min="25" max="29" width="3" style="38" customWidth="1"/>
+    <col min="30" max="30" width="3.6640625" style="38" customWidth="1"/>
+    <col min="31" max="31" width="3.33203125" style="38" customWidth="1"/>
+    <col min="32" max="32" width="3.1640625" style="38" customWidth="1"/>
     <col min="33" max="33" width="3" style="38" customWidth="1"/>
-    <col min="34" max="42" width="3.375" style="38" customWidth="1"/>
+    <col min="34" max="42" width="3.33203125" style="38" customWidth="1"/>
     <col min="43" max="44" width="3" style="38" customWidth="1"/>
-    <col min="45" max="46" width="3.375" style="38" customWidth="1"/>
-    <col min="47" max="47" width="3.875" style="38" customWidth="1"/>
-    <col min="48" max="48" width="4.375" style="38" customWidth="1"/>
-    <col min="49" max="49" width="3.125" style="38" customWidth="1"/>
+    <col min="45" max="46" width="3.33203125" style="38" customWidth="1"/>
+    <col min="47" max="47" width="3.83203125" style="38" customWidth="1"/>
+    <col min="48" max="48" width="4.33203125" style="38" customWidth="1"/>
+    <col min="49" max="49" width="3.1640625" style="38" customWidth="1"/>
     <col min="50" max="50" width="3.5" style="38" customWidth="1"/>
     <col min="51" max="51" width="3" style="38" customWidth="1"/>
-    <col min="52" max="54" width="3.375" style="38" customWidth="1"/>
-    <col min="55" max="59" width="3" style="38" customWidth="1"/>
-    <col min="60" max="60" width="3.125" style="38" customWidth="1"/>
-    <col min="61" max="63" width="3" style="38" customWidth="1"/>
-    <col min="64" max="75" width="3.375" style="38" customWidth="1"/>
-    <col min="76" max="76" width="3.125" style="38" customWidth="1"/>
+    <col min="52" max="54" width="3.33203125" style="38" customWidth="1"/>
+    <col min="55" max="56" width="3" style="38" customWidth="1"/>
+    <col min="57" max="57" width="4.33203125" style="38" customWidth="1"/>
+    <col min="58" max="58" width="4.1640625" style="38" customWidth="1"/>
+    <col min="59" max="59" width="4" style="38" customWidth="1"/>
+    <col min="60" max="60" width="3.1640625" style="38" customWidth="1"/>
+    <col min="61" max="63" width="3.5" style="38" bestFit="1" customWidth="1"/>
+    <col min="64" max="75" width="3.33203125" style="38" customWidth="1"/>
+    <col min="76" max="76" width="3.1640625" style="38" customWidth="1"/>
     <col min="77" max="78" width="3" style="38" customWidth="1"/>
-    <col min="79" max="85" width="3.375" style="38" customWidth="1"/>
+    <col min="79" max="85" width="3.33203125" style="38" customWidth="1"/>
     <col min="86" max="87" width="3" style="38" customWidth="1"/>
-    <col min="88" max="88" width="3.125" style="38" customWidth="1"/>
-    <col min="89" max="94" width="3" style="38" customWidth="1"/>
-    <col min="95" max="96" width="3.375" style="38" customWidth="1"/>
+    <col min="88" max="88" width="3.1640625" style="38" customWidth="1"/>
+    <col min="89" max="89" width="3" style="38" customWidth="1"/>
+    <col min="90" max="96" width="3.5" style="38" bestFit="1" customWidth="1"/>
     <col min="97" max="16384" width="12" style="38"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:96" ht="23.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="118" t="s">
+    <row r="1" spans="1:96" ht="23.45" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A1" s="98" t="s">
         <v>99</v>
       </c>
-      <c r="B1" s="118"/>
-      <c r="C1" s="120" t="s">
+      <c r="B1" s="98"/>
+      <c r="C1" s="100" t="s">
         <v>105</v>
       </c>
-      <c r="D1" s="122" t="s">
+      <c r="D1" s="102" t="s">
         <v>110</v>
       </c>
-      <c r="E1" s="120" t="s">
+      <c r="E1" s="100" t="s">
         <v>100</v>
       </c>
       <c r="F1" s="104" t="s">
@@ -2512,12 +2517,12 @@
       <c r="CQ1" s="108"/>
       <c r="CR1" s="81"/>
     </row>
-    <row r="2" spans="1:96" ht="39.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="119"/>
-      <c r="B2" s="119"/>
-      <c r="C2" s="120"/>
-      <c r="D2" s="122"/>
-      <c r="E2" s="120"/>
+    <row r="2" spans="1:96" ht="39.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A2" s="99"/>
+      <c r="B2" s="99"/>
+      <c r="C2" s="100"/>
+      <c r="D2" s="102"/>
+      <c r="E2" s="100"/>
       <c r="F2" s="39" t="s">
         <v>166</v>
       </c>
@@ -2792,14 +2797,14 @@
         <v>165</v>
       </c>
     </row>
-    <row r="3" spans="1:96" ht="24" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="99" t="s">
+    <row r="3" spans="1:96" ht="24" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A3" s="116" t="s">
         <v>221</v>
       </c>
-      <c r="B3" s="100"/>
-      <c r="C3" s="120"/>
-      <c r="D3" s="122"/>
-      <c r="E3" s="120"/>
+      <c r="B3" s="117"/>
+      <c r="C3" s="100"/>
+      <c r="D3" s="102"/>
+      <c r="E3" s="100"/>
       <c r="F3" s="39">
         <v>2</v>
       </c>
@@ -3162,131 +3167,131 @@
         <v>31</v>
       </c>
     </row>
-    <row r="4" spans="1:96" ht="24.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A4" s="101"/>
-      <c r="B4" s="102"/>
-      <c r="C4" s="121"/>
-      <c r="D4" s="123"/>
-      <c r="E4" s="121"/>
-      <c r="F4" s="109" t="s">
+    <row r="4" spans="1:96" ht="24.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A4" s="118"/>
+      <c r="B4" s="119"/>
+      <c r="C4" s="101"/>
+      <c r="D4" s="103"/>
+      <c r="E4" s="101"/>
+      <c r="F4" s="111" t="s">
         <v>167</v>
       </c>
-      <c r="G4" s="110"/>
-      <c r="H4" s="110"/>
-      <c r="I4" s="111"/>
+      <c r="G4" s="112"/>
+      <c r="H4" s="112"/>
+      <c r="I4" s="113"/>
       <c r="J4" s="41"/>
       <c r="K4" s="41"/>
-      <c r="L4" s="112" t="s">
+      <c r="L4" s="95" t="s">
         <v>232</v>
       </c>
-      <c r="M4" s="113"/>
-      <c r="N4" s="113"/>
-      <c r="O4" s="113"/>
-      <c r="P4" s="114"/>
+      <c r="M4" s="96"/>
+      <c r="N4" s="96"/>
+      <c r="O4" s="96"/>
+      <c r="P4" s="97"/>
       <c r="Q4" s="42"/>
       <c r="R4" s="42"/>
-      <c r="S4" s="112" t="s">
+      <c r="S4" s="95" t="s">
         <v>168</v>
       </c>
-      <c r="T4" s="113"/>
-      <c r="U4" s="113"/>
-      <c r="V4" s="113"/>
-      <c r="W4" s="114"/>
+      <c r="T4" s="96"/>
+      <c r="U4" s="96"/>
+      <c r="V4" s="96"/>
+      <c r="W4" s="97"/>
       <c r="X4" s="42"/>
       <c r="Y4" s="42"/>
-      <c r="Z4" s="112" t="s">
+      <c r="Z4" s="95" t="s">
         <v>169</v>
       </c>
-      <c r="AA4" s="113"/>
-      <c r="AB4" s="113"/>
-      <c r="AC4" s="113"/>
-      <c r="AD4" s="114"/>
+      <c r="AA4" s="96"/>
+      <c r="AB4" s="96"/>
+      <c r="AC4" s="96"/>
+      <c r="AD4" s="97"/>
       <c r="AE4" s="42"/>
       <c r="AF4" s="42"/>
-      <c r="AG4" s="112" t="s">
+      <c r="AG4" s="95" t="s">
         <v>170</v>
       </c>
-      <c r="AH4" s="113"/>
-      <c r="AI4" s="113"/>
-      <c r="AJ4" s="113"/>
-      <c r="AK4" s="114"/>
+      <c r="AH4" s="96"/>
+      <c r="AI4" s="96"/>
+      <c r="AJ4" s="96"/>
+      <c r="AK4" s="97"/>
       <c r="AL4" s="42"/>
       <c r="AM4" s="42"/>
-      <c r="AN4" s="112" t="s">
+      <c r="AN4" s="95" t="s">
         <v>171</v>
       </c>
-      <c r="AO4" s="113"/>
-      <c r="AP4" s="113"/>
-      <c r="AQ4" s="113"/>
-      <c r="AR4" s="114"/>
+      <c r="AO4" s="96"/>
+      <c r="AP4" s="96"/>
+      <c r="AQ4" s="96"/>
+      <c r="AR4" s="97"/>
       <c r="AS4" s="42"/>
       <c r="AT4" s="42"/>
-      <c r="AU4" s="112" t="s">
+      <c r="AU4" s="95" t="s">
         <v>172</v>
       </c>
-      <c r="AV4" s="113"/>
-      <c r="AW4" s="113"/>
-      <c r="AX4" s="113"/>
-      <c r="AY4" s="114"/>
+      <c r="AV4" s="96"/>
+      <c r="AW4" s="96"/>
+      <c r="AX4" s="96"/>
+      <c r="AY4" s="97"/>
       <c r="AZ4" s="42"/>
       <c r="BA4" s="42"/>
-      <c r="BB4" s="112" t="s">
+      <c r="BB4" s="95" t="s">
         <v>173</v>
       </c>
-      <c r="BC4" s="113"/>
-      <c r="BD4" s="113"/>
-      <c r="BE4" s="113"/>
-      <c r="BF4" s="114"/>
+      <c r="BC4" s="96"/>
+      <c r="BD4" s="96"/>
+      <c r="BE4" s="96"/>
+      <c r="BF4" s="97"/>
       <c r="BG4" s="42"/>
       <c r="BH4" s="42"/>
-      <c r="BI4" s="112" t="s">
+      <c r="BI4" s="95" t="s">
         <v>174</v>
       </c>
-      <c r="BJ4" s="113"/>
-      <c r="BK4" s="113"/>
-      <c r="BL4" s="113"/>
-      <c r="BM4" s="114"/>
+      <c r="BJ4" s="96"/>
+      <c r="BK4" s="96"/>
+      <c r="BL4" s="96"/>
+      <c r="BM4" s="97"/>
       <c r="BN4" s="42"/>
       <c r="BO4" s="42"/>
-      <c r="BP4" s="112" t="s">
+      <c r="BP4" s="95" t="s">
         <v>175</v>
       </c>
-      <c r="BQ4" s="113"/>
-      <c r="BR4" s="113"/>
-      <c r="BS4" s="113"/>
-      <c r="BT4" s="114"/>
+      <c r="BQ4" s="96"/>
+      <c r="BR4" s="96"/>
+      <c r="BS4" s="96"/>
+      <c r="BT4" s="97"/>
       <c r="BU4" s="42"/>
       <c r="BV4" s="42"/>
-      <c r="BW4" s="112" t="s">
+      <c r="BW4" s="95" t="s">
         <v>176</v>
       </c>
-      <c r="BX4" s="113"/>
-      <c r="BY4" s="113"/>
-      <c r="BZ4" s="113"/>
-      <c r="CA4" s="114"/>
+      <c r="BX4" s="96"/>
+      <c r="BY4" s="96"/>
+      <c r="BZ4" s="96"/>
+      <c r="CA4" s="97"/>
       <c r="CB4" s="42"/>
       <c r="CC4" s="42"/>
-      <c r="CD4" s="112" t="s">
+      <c r="CD4" s="95" t="s">
         <v>177</v>
       </c>
-      <c r="CE4" s="113"/>
-      <c r="CF4" s="113"/>
-      <c r="CG4" s="113"/>
-      <c r="CH4" s="114"/>
+      <c r="CE4" s="96"/>
+      <c r="CF4" s="96"/>
+      <c r="CG4" s="96"/>
+      <c r="CH4" s="97"/>
       <c r="CI4" s="42"/>
       <c r="CJ4" s="42"/>
-      <c r="CK4" s="112" t="s">
+      <c r="CK4" s="95" t="s">
         <v>178</v>
       </c>
-      <c r="CL4" s="113"/>
-      <c r="CM4" s="113"/>
-      <c r="CN4" s="113"/>
-      <c r="CO4" s="114"/>
+      <c r="CL4" s="96"/>
+      <c r="CM4" s="96"/>
+      <c r="CN4" s="96"/>
+      <c r="CO4" s="97"/>
       <c r="CP4" s="42"/>
       <c r="CQ4" s="42"/>
       <c r="CR4" s="78"/>
     </row>
-    <row r="5" spans="1:96" ht="13.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:96" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A5" s="44"/>
       <c r="B5" s="45" t="s">
         <v>219</v>
@@ -3388,7 +3393,7 @@
       <c r="CQ5" s="42"/>
       <c r="CR5" s="78"/>
     </row>
-    <row r="6" spans="1:96" ht="21" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:96" ht="21" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A6" s="72" t="s">
         <v>181</v>
       </c>
@@ -3494,7 +3499,7 @@
       <c r="CQ6" s="43"/>
       <c r="CR6" s="43"/>
     </row>
-    <row r="7" spans="1:96" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:96" x14ac:dyDescent="0.2">
       <c r="A7" s="43">
         <v>1.01</v>
       </c>
@@ -3504,10 +3509,10 @@
       <c r="C7" s="39" t="s">
         <v>107</v>
       </c>
-      <c r="D7" s="97" t="s">
+      <c r="D7" s="114" t="s">
         <v>222</v>
       </c>
-      <c r="E7" s="103"/>
+      <c r="E7" s="120"/>
       <c r="F7" s="43"/>
       <c r="G7" s="43"/>
       <c r="H7" s="43"/>
@@ -3600,7 +3605,7 @@
       <c r="CQ7" s="43"/>
       <c r="CR7" s="43"/>
     </row>
-    <row r="8" spans="1:96" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:96" x14ac:dyDescent="0.2">
       <c r="A8" s="43">
         <v>1.02</v>
       </c>
@@ -3610,10 +3615,10 @@
       <c r="C8" s="39" t="s">
         <v>108</v>
       </c>
-      <c r="D8" s="97" t="s">
+      <c r="D8" s="114" t="s">
         <v>222</v>
       </c>
-      <c r="E8" s="103"/>
+      <c r="E8" s="120"/>
       <c r="F8" s="43"/>
       <c r="G8" s="43"/>
       <c r="H8" s="43"/>
@@ -3706,7 +3711,7 @@
       <c r="CQ8" s="43"/>
       <c r="CR8" s="43"/>
     </row>
-    <row r="9" spans="1:96" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:96" x14ac:dyDescent="0.2">
       <c r="A9" s="43">
         <v>1.03</v>
       </c>
@@ -3716,10 +3721,10 @@
       <c r="C9" s="39" t="s">
         <v>108</v>
       </c>
-      <c r="D9" s="97" t="s">
+      <c r="D9" s="114" t="s">
         <v>222</v>
       </c>
-      <c r="E9" s="103"/>
+      <c r="E9" s="120"/>
       <c r="F9" s="43"/>
       <c r="G9" s="43"/>
       <c r="H9" s="43"/>
@@ -3812,7 +3817,7 @@
       <c r="CQ9" s="43"/>
       <c r="CR9" s="43"/>
     </row>
-    <row r="10" spans="1:96" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:96" x14ac:dyDescent="0.2">
       <c r="A10" s="43">
         <v>1.04</v>
       </c>
@@ -3822,10 +3827,10 @@
       <c r="C10" s="39" t="s">
         <v>108</v>
       </c>
-      <c r="D10" s="97" t="s">
+      <c r="D10" s="114" t="s">
         <v>222</v>
       </c>
-      <c r="E10" s="103"/>
+      <c r="E10" s="120"/>
       <c r="F10" s="43"/>
       <c r="G10" s="43"/>
       <c r="H10" s="43"/>
@@ -3918,7 +3923,7 @@
       <c r="CQ10" s="43"/>
       <c r="CR10" s="43"/>
     </row>
-    <row r="11" spans="1:96" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:96" x14ac:dyDescent="0.2">
       <c r="A11" s="74" t="s">
         <v>180</v>
       </c>
@@ -4024,7 +4029,7 @@
       <c r="CQ11" s="43"/>
       <c r="CR11" s="43"/>
     </row>
-    <row r="12" spans="1:96" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:96" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A12" s="53">
         <v>2</v>
       </c>
@@ -4126,7 +4131,7 @@
       <c r="CQ12" s="43"/>
       <c r="CR12" s="43"/>
     </row>
-    <row r="13" spans="1:96" ht="31.8" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:96" ht="31.9" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A13" s="43"/>
       <c r="B13" s="56" t="s">
         <v>106</v>
@@ -4228,7 +4233,7 @@
       <c r="CQ13" s="43"/>
       <c r="CR13" s="43"/>
     </row>
-    <row r="14" spans="1:96" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:96" x14ac:dyDescent="0.2">
       <c r="A14" s="43">
         <v>2.0099999999999998</v>
       </c>
@@ -4332,7 +4337,7 @@
       <c r="CQ14" s="43"/>
       <c r="CR14" s="43"/>
     </row>
-    <row r="15" spans="1:96" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:96" x14ac:dyDescent="0.2">
       <c r="A15" s="43">
         <v>2.02</v>
       </c>
@@ -4436,7 +4441,7 @@
       <c r="CQ15" s="43"/>
       <c r="CR15" s="43"/>
     </row>
-    <row r="16" spans="1:96" ht="20.399999999999999" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:96" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A16" s="43">
         <v>2.0299999999999998</v>
       </c>
@@ -4540,7 +4545,7 @@
       <c r="CQ16" s="43"/>
       <c r="CR16" s="43"/>
     </row>
-    <row r="17" spans="1:96" ht="20.399999999999999" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:96" ht="38.25" x14ac:dyDescent="0.2">
       <c r="A17" s="43">
         <v>2.04</v>
       </c>
@@ -4644,7 +4649,7 @@
       <c r="CQ17" s="43"/>
       <c r="CR17" s="43"/>
     </row>
-    <row r="18" spans="1:96" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:96" x14ac:dyDescent="0.2">
       <c r="A18" s="43">
         <v>2.0499999999999998</v>
       </c>
@@ -4748,7 +4753,7 @@
       <c r="CQ18" s="43"/>
       <c r="CR18" s="43"/>
     </row>
-    <row r="19" spans="1:96" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:96" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A19" s="53">
         <v>3</v>
       </c>
@@ -4850,7 +4855,7 @@
       <c r="CQ19" s="43"/>
       <c r="CR19" s="43"/>
     </row>
-    <row r="20" spans="1:96" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:96" x14ac:dyDescent="0.2">
       <c r="A20" s="43">
         <v>3.01</v>
       </c>
@@ -4954,7 +4959,7 @@
       <c r="CQ20" s="43"/>
       <c r="CR20" s="43"/>
     </row>
-    <row r="21" spans="1:96" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:96" x14ac:dyDescent="0.2">
       <c r="A21" s="43">
         <v>3.02</v>
       </c>
@@ -5058,7 +5063,7 @@
       <c r="CQ21" s="43"/>
       <c r="CR21" s="43"/>
     </row>
-    <row r="22" spans="1:96" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:96" x14ac:dyDescent="0.2">
       <c r="A22" s="43">
         <v>3.03</v>
       </c>
@@ -5162,7 +5167,7 @@
       <c r="CQ22" s="43"/>
       <c r="CR22" s="43"/>
     </row>
-    <row r="23" spans="1:96" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:96" x14ac:dyDescent="0.2">
       <c r="A23" s="43">
         <v>3.04</v>
       </c>
@@ -5266,7 +5271,7 @@
       <c r="CQ23" s="43"/>
       <c r="CR23" s="43"/>
     </row>
-    <row r="24" spans="1:96" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:96" x14ac:dyDescent="0.2">
       <c r="A24" s="43">
         <v>3.05</v>
       </c>
@@ -5370,7 +5375,7 @@
       <c r="CQ24" s="43"/>
       <c r="CR24" s="43"/>
     </row>
-    <row r="25" spans="1:96" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:96" x14ac:dyDescent="0.2">
       <c r="A25" s="43">
         <v>3.06</v>
       </c>
@@ -5474,7 +5479,7 @@
       <c r="CQ25" s="43"/>
       <c r="CR25" s="43"/>
     </row>
-    <row r="26" spans="1:96" ht="31.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:96" ht="31.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A26" s="43">
         <v>3.07</v>
       </c>
@@ -5578,7 +5583,7 @@
       <c r="CQ26" s="43"/>
       <c r="CR26" s="43"/>
     </row>
-    <row r="27" spans="1:96" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:96" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A27" s="43">
         <v>3.08</v>
       </c>
@@ -5682,7 +5687,7 @@
       <c r="CQ27" s="43"/>
       <c r="CR27" s="43"/>
     </row>
-    <row r="28" spans="1:96" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:96" x14ac:dyDescent="0.2">
       <c r="A28" s="43">
         <v>3.09</v>
       </c>
@@ -5786,7 +5791,7 @@
       <c r="CQ28" s="43"/>
       <c r="CR28" s="43"/>
     </row>
-    <row r="29" spans="1:96" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:96" x14ac:dyDescent="0.2">
       <c r="A29" s="61">
         <v>3.1</v>
       </c>
@@ -5890,7 +5895,7 @@
       <c r="CQ29" s="43"/>
       <c r="CR29" s="43"/>
     </row>
-    <row r="30" spans="1:96" ht="20.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:96" ht="20.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A30" s="53">
         <v>4</v>
       </c>
@@ -5992,7 +5997,7 @@
       <c r="CQ30" s="43"/>
       <c r="CR30" s="43"/>
     </row>
-    <row r="31" spans="1:96" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:96" x14ac:dyDescent="0.2">
       <c r="A31" s="43">
         <v>4.01</v>
       </c>
@@ -6095,7 +6100,7 @@
       <c r="CQ31" s="43"/>
       <c r="CR31" s="43"/>
     </row>
-    <row r="32" spans="1:96" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:96" x14ac:dyDescent="0.2">
       <c r="A32" s="43">
         <v>4.0199999999999996</v>
       </c>
@@ -6198,7 +6203,7 @@
       <c r="CQ32" s="43"/>
       <c r="CR32" s="43"/>
     </row>
-    <row r="33" spans="1:96" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:96" x14ac:dyDescent="0.2">
       <c r="A33" s="43">
         <v>4.03</v>
       </c>
@@ -6301,7 +6306,7 @@
       <c r="CQ33" s="43"/>
       <c r="CR33" s="43"/>
     </row>
-    <row r="34" spans="1:96" ht="22.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:96" ht="22.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A34" s="53">
         <v>5</v>
       </c>
@@ -6403,7 +6408,7 @@
       <c r="CQ34" s="43"/>
       <c r="CR34" s="43"/>
     </row>
-    <row r="35" spans="1:96" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:96" x14ac:dyDescent="0.2">
       <c r="A35" s="43">
         <v>5.01</v>
       </c>
@@ -6506,7 +6511,7 @@
       <c r="CQ35" s="43"/>
       <c r="CR35" s="43"/>
     </row>
-    <row r="36" spans="1:96" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:96" x14ac:dyDescent="0.2">
       <c r="A36" s="43">
         <v>5.0199999999999996</v>
       </c>
@@ -6610,7 +6615,7 @@
       <c r="CQ36" s="43"/>
       <c r="CR36" s="43"/>
     </row>
-    <row r="37" spans="1:96" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:96" x14ac:dyDescent="0.2">
       <c r="A37" s="43">
         <v>5.03</v>
       </c>
@@ -6714,7 +6719,7 @@
       <c r="CQ37" s="43"/>
       <c r="CR37" s="43"/>
     </row>
-    <row r="38" spans="1:96" ht="24" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:96" ht="24" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A38" s="50" t="s">
         <v>192</v>
       </c>
@@ -6820,7 +6825,7 @@
       <c r="CQ38" s="43"/>
       <c r="CR38" s="43"/>
     </row>
-    <row r="39" spans="1:96" ht="21.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:96" ht="21.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A39" s="53">
         <v>6</v>
       </c>
@@ -6922,7 +6927,7 @@
       <c r="CQ39" s="43"/>
       <c r="CR39" s="43"/>
     </row>
-    <row r="40" spans="1:96" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:96" x14ac:dyDescent="0.2">
       <c r="A40" s="43">
         <v>6.01</v>
       </c>
@@ -6963,7 +6968,9 @@
       <c r="AF40" s="43"/>
       <c r="AG40" s="43"/>
       <c r="AH40" s="43"/>
-      <c r="AI40" s="89"/>
+      <c r="AI40" s="89">
+        <v>1</v>
+      </c>
       <c r="AJ40" s="43"/>
       <c r="AK40" s="43"/>
       <c r="AL40" s="43"/>
@@ -7026,7 +7033,7 @@
       <c r="CQ40" s="43"/>
       <c r="CR40" s="43"/>
     </row>
-    <row r="41" spans="1:96" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:96" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A41" s="53">
         <v>7</v>
       </c>
@@ -7128,7 +7135,7 @@
       <c r="CQ41" s="43"/>
       <c r="CR41" s="43"/>
     </row>
-    <row r="42" spans="1:96" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:96" x14ac:dyDescent="0.2">
       <c r="A42" s="43">
         <v>7.01</v>
       </c>
@@ -7232,7 +7239,7 @@
       <c r="CQ42" s="43"/>
       <c r="CR42" s="43"/>
     </row>
-    <row r="43" spans="1:96" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:96" x14ac:dyDescent="0.2">
       <c r="A43" s="43">
         <v>7.02</v>
       </c>
@@ -7336,7 +7343,7 @@
       <c r="CQ43" s="43"/>
       <c r="CR43" s="43"/>
     </row>
-    <row r="44" spans="1:96" x14ac:dyDescent="0.3">
+    <row r="44" spans="1:96" x14ac:dyDescent="0.2">
       <c r="A44" s="43">
         <v>7.03</v>
       </c>
@@ -7440,7 +7447,7 @@
       <c r="CQ44" s="43"/>
       <c r="CR44" s="43"/>
     </row>
-    <row r="45" spans="1:96" x14ac:dyDescent="0.3">
+    <row r="45" spans="1:96" x14ac:dyDescent="0.2">
       <c r="A45" s="43">
         <v>7.04</v>
       </c>
@@ -7544,7 +7551,7 @@
       <c r="CQ45" s="43"/>
       <c r="CR45" s="43"/>
     </row>
-    <row r="46" spans="1:96" x14ac:dyDescent="0.3">
+    <row r="46" spans="1:96" x14ac:dyDescent="0.2">
       <c r="A46" s="43">
         <v>7.05</v>
       </c>
@@ -7648,7 +7655,7 @@
       <c r="CQ46" s="43"/>
       <c r="CR46" s="43"/>
     </row>
-    <row r="47" spans="1:96" x14ac:dyDescent="0.3">
+    <row r="47" spans="1:96" x14ac:dyDescent="0.2">
       <c r="A47" s="43">
         <v>7.06</v>
       </c>
@@ -7752,7 +7759,7 @@
       <c r="CQ47" s="43"/>
       <c r="CR47" s="43"/>
     </row>
-    <row r="48" spans="1:96" ht="21.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="48" spans="1:96" ht="21.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A48" s="53">
         <v>8</v>
       </c>
@@ -7854,7 +7861,7 @@
       <c r="CQ48" s="43"/>
       <c r="CR48" s="43"/>
     </row>
-    <row r="49" spans="1:96" x14ac:dyDescent="0.3">
+    <row r="49" spans="1:96" x14ac:dyDescent="0.2">
       <c r="A49" s="43">
         <v>8.01</v>
       </c>
@@ -7958,7 +7965,7 @@
       <c r="CQ49" s="43"/>
       <c r="CR49" s="43"/>
     </row>
-    <row r="50" spans="1:96" x14ac:dyDescent="0.3">
+    <row r="50" spans="1:96" x14ac:dyDescent="0.2">
       <c r="A50" s="43">
         <v>8.02</v>
       </c>
@@ -8062,7 +8069,7 @@
       <c r="CQ50" s="43"/>
       <c r="CR50" s="43"/>
     </row>
-    <row r="51" spans="1:96" x14ac:dyDescent="0.3">
+    <row r="51" spans="1:96" x14ac:dyDescent="0.2">
       <c r="A51" s="43">
         <v>8.0299999999999994</v>
       </c>
@@ -8166,7 +8173,7 @@
       <c r="CQ51" s="43"/>
       <c r="CR51" s="43"/>
     </row>
-    <row r="52" spans="1:96" x14ac:dyDescent="0.3">
+    <row r="52" spans="1:96" x14ac:dyDescent="0.2">
       <c r="A52" s="43">
         <v>8.0399999999999991</v>
       </c>
@@ -8270,7 +8277,7 @@
       <c r="CQ52" s="43"/>
       <c r="CR52" s="43"/>
     </row>
-    <row r="53" spans="1:96" x14ac:dyDescent="0.3">
+    <row r="53" spans="1:96" x14ac:dyDescent="0.2">
       <c r="A53" s="43">
         <v>8.0500000000000007</v>
       </c>
@@ -8374,7 +8381,7 @@
       <c r="CQ53" s="43"/>
       <c r="CR53" s="43"/>
     </row>
-    <row r="54" spans="1:96" x14ac:dyDescent="0.3">
+    <row r="54" spans="1:96" x14ac:dyDescent="0.2">
       <c r="A54" s="43">
         <v>8.06</v>
       </c>
@@ -8478,7 +8485,7 @@
       <c r="CQ54" s="43"/>
       <c r="CR54" s="43"/>
     </row>
-    <row r="55" spans="1:96" ht="22.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="55" spans="1:96" ht="22.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A55" s="53">
         <v>9</v>
       </c>
@@ -8580,7 +8587,7 @@
       <c r="CQ55" s="43"/>
       <c r="CR55" s="43"/>
     </row>
-    <row r="56" spans="1:96" x14ac:dyDescent="0.3">
+    <row r="56" spans="1:96" x14ac:dyDescent="0.2">
       <c r="A56" s="43">
         <v>9.01</v>
       </c>
@@ -8684,7 +8691,7 @@
       <c r="CQ56" s="43"/>
       <c r="CR56" s="43"/>
     </row>
-    <row r="57" spans="1:96" x14ac:dyDescent="0.3">
+    <row r="57" spans="1:96" x14ac:dyDescent="0.2">
       <c r="A57" s="43">
         <v>9.02</v>
       </c>
@@ -8788,7 +8795,7 @@
       <c r="CQ57" s="43"/>
       <c r="CR57" s="43"/>
     </row>
-    <row r="58" spans="1:96" x14ac:dyDescent="0.3">
+    <row r="58" spans="1:96" x14ac:dyDescent="0.2">
       <c r="A58" s="43">
         <v>9.0299999999999994</v>
       </c>
@@ -8892,7 +8899,7 @@
       <c r="CQ58" s="43"/>
       <c r="CR58" s="43"/>
     </row>
-    <row r="59" spans="1:96" x14ac:dyDescent="0.3">
+    <row r="59" spans="1:96" x14ac:dyDescent="0.2">
       <c r="A59" s="43">
         <v>9.0399999999999991</v>
       </c>
@@ -8996,7 +9003,7 @@
       <c r="CQ59" s="43"/>
       <c r="CR59" s="43"/>
     </row>
-    <row r="60" spans="1:96" x14ac:dyDescent="0.3">
+    <row r="60" spans="1:96" x14ac:dyDescent="0.2">
       <c r="A60" s="43">
         <v>9.0500000000000007</v>
       </c>
@@ -9100,7 +9107,7 @@
       <c r="CQ60" s="43"/>
       <c r="CR60" s="43"/>
     </row>
-    <row r="61" spans="1:96" ht="31.2" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="61" spans="1:96" ht="31.15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A61" s="50" t="s">
         <v>194</v>
       </c>
@@ -9206,7 +9213,7 @@
       <c r="CQ61" s="43"/>
       <c r="CR61" s="43"/>
     </row>
-    <row r="62" spans="1:96" ht="23.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="62" spans="1:96" ht="23.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A62" s="53">
         <v>10</v>
       </c>
@@ -9308,7 +9315,7 @@
       <c r="CQ62" s="43"/>
       <c r="CR62" s="43"/>
     </row>
-    <row r="63" spans="1:96" x14ac:dyDescent="0.3">
+    <row r="63" spans="1:96" x14ac:dyDescent="0.2">
       <c r="A63" s="43">
         <v>10.01</v>
       </c>
@@ -9412,7 +9419,7 @@
       <c r="CQ63" s="43"/>
       <c r="CR63" s="43"/>
     </row>
-    <row r="64" spans="1:96" x14ac:dyDescent="0.3">
+    <row r="64" spans="1:96" x14ac:dyDescent="0.2">
       <c r="A64" s="43">
         <v>10.02</v>
       </c>
@@ -9516,7 +9523,7 @@
       <c r="CQ64" s="43"/>
       <c r="CR64" s="43"/>
     </row>
-    <row r="65" spans="1:96" x14ac:dyDescent="0.3">
+    <row r="65" spans="1:96" x14ac:dyDescent="0.2">
       <c r="A65" s="43">
         <v>10.029999999999999</v>
       </c>
@@ -9620,7 +9627,7 @@
       <c r="CQ65" s="43"/>
       <c r="CR65" s="43"/>
     </row>
-    <row r="66" spans="1:96" x14ac:dyDescent="0.3">
+    <row r="66" spans="1:96" x14ac:dyDescent="0.2">
       <c r="A66" s="43">
         <v>10.039999999999999</v>
       </c>
@@ -9724,7 +9731,7 @@
       <c r="CQ66" s="43"/>
       <c r="CR66" s="43"/>
     </row>
-    <row r="67" spans="1:96" x14ac:dyDescent="0.3">
+    <row r="67" spans="1:96" x14ac:dyDescent="0.2">
       <c r="A67" s="43">
         <v>10.050000000000001</v>
       </c>
@@ -9828,7 +9835,7 @@
       <c r="CQ67" s="43"/>
       <c r="CR67" s="43"/>
     </row>
-    <row r="68" spans="1:96" ht="21.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="68" spans="1:96" ht="21.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A68" s="53">
         <v>11</v>
       </c>
@@ -9930,7 +9937,7 @@
       <c r="CQ68" s="43"/>
       <c r="CR68" s="43"/>
     </row>
-    <row r="69" spans="1:96" x14ac:dyDescent="0.3">
+    <row r="69" spans="1:96" x14ac:dyDescent="0.2">
       <c r="A69" s="43">
         <v>11.01</v>
       </c>
@@ -10034,7 +10041,7 @@
       <c r="CQ69" s="43"/>
       <c r="CR69" s="43"/>
     </row>
-    <row r="70" spans="1:96" x14ac:dyDescent="0.3">
+    <row r="70" spans="1:96" x14ac:dyDescent="0.2">
       <c r="A70" s="43">
         <v>11.02</v>
       </c>
@@ -10138,7 +10145,7 @@
       <c r="CQ70" s="43"/>
       <c r="CR70" s="43"/>
     </row>
-    <row r="71" spans="1:96" x14ac:dyDescent="0.3">
+    <row r="71" spans="1:96" x14ac:dyDescent="0.2">
       <c r="A71" s="43">
         <v>11.03</v>
       </c>
@@ -10242,7 +10249,7 @@
       <c r="CQ71" s="43"/>
       <c r="CR71" s="43"/>
     </row>
-    <row r="72" spans="1:96" x14ac:dyDescent="0.3">
+    <row r="72" spans="1:96" x14ac:dyDescent="0.2">
       <c r="A72" s="43">
         <v>11.04</v>
       </c>
@@ -10346,7 +10353,7 @@
       <c r="CQ72" s="43"/>
       <c r="CR72" s="43"/>
     </row>
-    <row r="73" spans="1:96" x14ac:dyDescent="0.3">
+    <row r="73" spans="1:96" x14ac:dyDescent="0.2">
       <c r="A73" s="43">
         <v>11.05</v>
       </c>
@@ -10450,7 +10457,7 @@
       <c r="CQ73" s="43"/>
       <c r="CR73" s="43"/>
     </row>
-    <row r="74" spans="1:96" ht="24" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="74" spans="1:96" ht="24" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A74" s="53">
         <v>12</v>
       </c>
@@ -10552,7 +10559,7 @@
       <c r="CQ74" s="43"/>
       <c r="CR74" s="43"/>
     </row>
-    <row r="75" spans="1:96" x14ac:dyDescent="0.3">
+    <row r="75" spans="1:96" x14ac:dyDescent="0.2">
       <c r="A75" s="43">
         <v>12.01</v>
       </c>
@@ -10656,7 +10663,7 @@
       <c r="CQ75" s="43"/>
       <c r="CR75" s="43"/>
     </row>
-    <row r="76" spans="1:96" x14ac:dyDescent="0.3">
+    <row r="76" spans="1:96" x14ac:dyDescent="0.2">
       <c r="A76" s="43">
         <v>12.02</v>
       </c>
@@ -10760,7 +10767,7 @@
       <c r="CQ76" s="43"/>
       <c r="CR76" s="43"/>
     </row>
-    <row r="77" spans="1:96" ht="20.399999999999999" x14ac:dyDescent="0.3">
+    <row r="77" spans="1:96" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A77" s="43">
         <v>12.03</v>
       </c>
@@ -10864,7 +10871,7 @@
       <c r="CQ77" s="43"/>
       <c r="CR77" s="43"/>
     </row>
-    <row r="78" spans="1:96" x14ac:dyDescent="0.3">
+    <row r="78" spans="1:96" x14ac:dyDescent="0.2">
       <c r="A78" s="43">
         <v>12.04</v>
       </c>
@@ -10968,7 +10975,7 @@
       <c r="CQ78" s="43"/>
       <c r="CR78" s="43"/>
     </row>
-    <row r="79" spans="1:96" x14ac:dyDescent="0.3">
+    <row r="79" spans="1:96" x14ac:dyDescent="0.2">
       <c r="A79" s="43">
         <v>12.05</v>
       </c>
@@ -11072,7 +11079,7 @@
       <c r="CQ79" s="43"/>
       <c r="CR79" s="43"/>
     </row>
-    <row r="80" spans="1:96" ht="23.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="80" spans="1:96" ht="23.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A80" s="53">
         <v>13</v>
       </c>
@@ -11174,7 +11181,7 @@
       <c r="CQ80" s="43"/>
       <c r="CR80" s="43"/>
     </row>
-    <row r="81" spans="1:96" x14ac:dyDescent="0.3">
+    <row r="81" spans="1:96" x14ac:dyDescent="0.2">
       <c r="A81" s="43">
         <v>13.01</v>
       </c>
@@ -11278,7 +11285,7 @@
       <c r="CQ81" s="43"/>
       <c r="CR81" s="43"/>
     </row>
-    <row r="82" spans="1:96" ht="21.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="82" spans="1:96" ht="21.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A82" s="53">
         <v>14</v>
       </c>
@@ -11380,7 +11387,7 @@
       <c r="CQ82" s="43"/>
       <c r="CR82" s="43"/>
     </row>
-    <row r="83" spans="1:96" x14ac:dyDescent="0.3">
+    <row r="83" spans="1:96" x14ac:dyDescent="0.2">
       <c r="A83" s="43">
         <v>14.01</v>
       </c>
@@ -11484,7 +11491,7 @@
       <c r="CQ83" s="43"/>
       <c r="CR83" s="43"/>
     </row>
-    <row r="84" spans="1:96" x14ac:dyDescent="0.3">
+    <row r="84" spans="1:96" x14ac:dyDescent="0.2">
       <c r="A84" s="53">
         <v>15</v>
       </c>
@@ -11586,7 +11593,7 @@
       <c r="CQ84" s="43"/>
       <c r="CR84" s="43"/>
     </row>
-    <row r="85" spans="1:96" x14ac:dyDescent="0.3">
+    <row r="85" spans="1:96" x14ac:dyDescent="0.2">
       <c r="A85" s="43">
         <v>17</v>
       </c>
@@ -11688,8 +11695,8 @@
       <c r="CQ85" s="43"/>
       <c r="CR85" s="80"/>
     </row>
-    <row r="87" spans="1:96" x14ac:dyDescent="0.3">
-      <c r="B87" s="97" t="s">
+    <row r="87" spans="1:96" x14ac:dyDescent="0.2">
+      <c r="B87" s="114" t="s">
         <v>195</v>
       </c>
       <c r="C87" s="70"/>
@@ -11706,8 +11713,8 @@
       <c r="J87" s="49"/>
       <c r="K87" s="49"/>
     </row>
-    <row r="88" spans="1:96" x14ac:dyDescent="0.3">
-      <c r="B88" s="98"/>
+    <row r="88" spans="1:96" x14ac:dyDescent="0.2">
+      <c r="B88" s="115"/>
       <c r="C88" s="49"/>
       <c r="D88" s="87">
         <f>+D11</f>
@@ -11718,15 +11725,15 @@
         <v>44074</v>
       </c>
     </row>
-    <row r="89" spans="1:96" x14ac:dyDescent="0.3">
-      <c r="B89" s="97" t="s">
+    <row r="89" spans="1:96" x14ac:dyDescent="0.2">
+      <c r="B89" s="114" t="s">
         <v>198</v>
       </c>
       <c r="C89" s="70"/>
-      <c r="D89" s="95" t="s">
+      <c r="D89" s="109" t="s">
         <v>233</v>
       </c>
-      <c r="E89" s="96"/>
+      <c r="E89" s="110"/>
       <c r="F89" s="64"/>
       <c r="G89" s="64"/>
       <c r="H89" s="64"/>
@@ -11734,13 +11741,13 @@
       <c r="J89" s="64"/>
       <c r="K89" s="64"/>
     </row>
-    <row r="90" spans="1:96" ht="25.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B90" s="98"/>
+    <row r="90" spans="1:96" ht="25.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B90" s="115"/>
       <c r="C90" s="71"/>
-      <c r="D90" s="95" t="s">
+      <c r="D90" s="109" t="s">
         <v>234</v>
       </c>
-      <c r="E90" s="96"/>
+      <c r="E90" s="110"/>
       <c r="F90" s="64"/>
       <c r="G90" s="64"/>
       <c r="H90" s="64"/>
@@ -11748,18 +11755,18 @@
       <c r="J90" s="64"/>
       <c r="K90" s="64"/>
     </row>
-    <row r="92" spans="1:96" x14ac:dyDescent="0.3">
+    <row r="92" spans="1:96" x14ac:dyDescent="0.2">
       <c r="C92" s="65">
         <f>13*5</f>
         <v>65</v>
       </c>
     </row>
-    <row r="95" spans="1:96" x14ac:dyDescent="0.3">
+    <row r="95" spans="1:96" x14ac:dyDescent="0.2">
       <c r="B95" s="91" t="s">
         <v>242</v>
       </c>
     </row>
-    <row r="96" spans="1:96" x14ac:dyDescent="0.3">
+    <row r="96" spans="1:96" x14ac:dyDescent="0.2">
       <c r="A96" s="38">
         <v>1</v>
       </c>
@@ -11767,7 +11774,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="97" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="97" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A97" s="38">
         <v>2</v>
       </c>
@@ -11775,7 +11782,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="98" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="98" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A98" s="38">
         <v>3</v>
       </c>
@@ -11783,7 +11790,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="99" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="99" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A99" s="38">
         <v>4</v>
       </c>
@@ -11791,7 +11798,7 @@
         <v>240</v>
       </c>
     </row>
-    <row r="100" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="100" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A100" s="38">
         <v>5</v>
       </c>
@@ -11799,7 +11806,7 @@
         <v>241</v>
       </c>
     </row>
-    <row r="101" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="101" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A101" s="38">
         <v>6</v>
       </c>
@@ -11807,7 +11814,7 @@
         <v>185</v>
       </c>
     </row>
-    <row r="102" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="102" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A102" s="38">
         <v>7</v>
       </c>
@@ -11817,6 +11824,19 @@
     </row>
   </sheetData>
   <mergeCells count="29">
+    <mergeCell ref="D90:E90"/>
+    <mergeCell ref="B89:B90"/>
+    <mergeCell ref="B87:B88"/>
+    <mergeCell ref="A3:B4"/>
+    <mergeCell ref="D9:E9"/>
+    <mergeCell ref="D10:E10"/>
+    <mergeCell ref="D7:E7"/>
+    <mergeCell ref="D8:E8"/>
+    <mergeCell ref="D89:E89"/>
+    <mergeCell ref="F4:I4"/>
+    <mergeCell ref="L4:P4"/>
+    <mergeCell ref="S4:W4"/>
+    <mergeCell ref="Z4:AD4"/>
     <mergeCell ref="BP4:BT4"/>
     <mergeCell ref="A1:B2"/>
     <mergeCell ref="E1:E4"/>
@@ -11825,11 +11845,6 @@
     <mergeCell ref="F1:AH1"/>
     <mergeCell ref="AI1:BM1"/>
     <mergeCell ref="BN1:CQ1"/>
-    <mergeCell ref="D89:E89"/>
-    <mergeCell ref="F4:I4"/>
-    <mergeCell ref="L4:P4"/>
-    <mergeCell ref="S4:W4"/>
-    <mergeCell ref="Z4:AD4"/>
     <mergeCell ref="BB4:BF4"/>
     <mergeCell ref="AU4:AY4"/>
     <mergeCell ref="AN4:AR4"/>
@@ -11838,14 +11853,6 @@
     <mergeCell ref="CK4:CO4"/>
     <mergeCell ref="CD4:CH4"/>
     <mergeCell ref="BW4:CA4"/>
-    <mergeCell ref="D90:E90"/>
-    <mergeCell ref="B89:B90"/>
-    <mergeCell ref="B87:B88"/>
-    <mergeCell ref="A3:B4"/>
-    <mergeCell ref="D9:E9"/>
-    <mergeCell ref="D10:E10"/>
-    <mergeCell ref="D7:E7"/>
-    <mergeCell ref="D8:E8"/>
   </mergeCells>
   <phoneticPr fontId="3" type="noConversion"/>
   <pageMargins left="0.70866141732283472" right="0.70866141732283472" top="0.74803149606299213" bottom="0.74803149606299213" header="0.31496062992125984" footer="0.31496062992125984"/>
@@ -11858,27 +11865,27 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CEAF0343-53AF-4B02-BC03-ACC3328D8F3B}">
   <dimension ref="A2:K59"/>
   <sheetViews>
-    <sheetView showGridLines="0" topLeftCell="A8" workbookViewId="0">
+    <sheetView showGridLines="0" topLeftCell="A52" workbookViewId="0">
       <selection activeCell="M25" sqref="M25"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="12" defaultRowHeight="13.8" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="12" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="5.875" style="1" customWidth="1"/>
-    <col min="2" max="2" width="38.875" style="1" customWidth="1"/>
-    <col min="3" max="3" width="44.375" style="1" hidden="1" customWidth="1"/>
+    <col min="1" max="1" width="5.83203125" style="1" customWidth="1"/>
+    <col min="2" max="2" width="38.83203125" style="1" customWidth="1"/>
+    <col min="3" max="3" width="44.33203125" style="1" hidden="1" customWidth="1"/>
     <col min="4" max="4" width="12.5" style="1" customWidth="1"/>
     <col min="5" max="5" width="11" style="1" customWidth="1"/>
-    <col min="6" max="6" width="12.125" style="1" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="12.1640625" style="1" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="13.5" style="1" customWidth="1"/>
     <col min="8" max="8" width="16" style="1" customWidth="1"/>
-    <col min="9" max="9" width="13.625" style="1" customWidth="1"/>
-    <col min="10" max="10" width="14.125" style="1" customWidth="1"/>
+    <col min="9" max="9" width="13.6640625" style="1" customWidth="1"/>
+    <col min="10" max="10" width="14.1640625" style="1" customWidth="1"/>
     <col min="11" max="11" width="14" style="1" customWidth="1"/>
     <col min="12" max="16384" width="12" style="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:11" ht="27.6" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:11" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A2" s="11" t="s">
         <v>4</v>
       </c>
@@ -11910,7 +11917,7 @@
         <v>160</v>
       </c>
     </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A3" s="2"/>
       <c r="B3" s="8" t="s">
         <v>19</v>
@@ -11928,7 +11935,7 @@
         <v>61500</v>
       </c>
     </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A4" s="16">
         <v>1</v>
       </c>
@@ -11966,7 +11973,7 @@
         <v>13500</v>
       </c>
     </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A5" s="2">
         <v>2</v>
       </c>
@@ -12006,7 +12013,7 @@
         <v>12000</v>
       </c>
     </row>
-    <row r="6" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A6" s="16">
         <v>3</v>
       </c>
@@ -12043,7 +12050,7 @@
         <v>8000</v>
       </c>
     </row>
-    <row r="7" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A7" s="16">
         <v>4</v>
       </c>
@@ -12080,7 +12087,7 @@
         <v>8000</v>
       </c>
     </row>
-    <row r="8" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A8" s="16">
         <v>5</v>
       </c>
@@ -12114,7 +12121,7 @@
         <v>4000</v>
       </c>
     </row>
-    <row r="9" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A9" s="16">
         <v>6</v>
       </c>
@@ -12149,7 +12156,7 @@
         <v>8000</v>
       </c>
     </row>
-    <row r="10" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A10" s="16">
         <v>7</v>
       </c>
@@ -12183,7 +12190,7 @@
         <v>4000</v>
       </c>
     </row>
-    <row r="11" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A11" s="16">
         <v>8</v>
       </c>
@@ -12217,7 +12224,7 @@
         <v>4000</v>
       </c>
     </row>
-    <row r="12" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A12" s="2"/>
       <c r="B12" s="9" t="s">
         <v>20</v>
@@ -12238,7 +12245,7 @@
         <v>5000</v>
       </c>
     </row>
-    <row r="13" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A13" s="2">
         <v>1</v>
       </c>
@@ -12275,7 +12282,7 @@
         <v>5000</v>
       </c>
     </row>
-    <row r="14" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A14" s="2"/>
       <c r="B14" s="8" t="s">
         <v>26</v>
@@ -12296,7 +12303,7 @@
         <v>8400</v>
       </c>
     </row>
-    <row r="15" spans="1:11" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:11" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A15" s="2">
         <v>1</v>
       </c>
@@ -12331,7 +12338,7 @@
         <v>2800</v>
       </c>
     </row>
-    <row r="16" spans="1:11" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:11" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A16" s="16">
         <v>2</v>
       </c>
@@ -12363,7 +12370,7 @@
         <v>2100</v>
       </c>
     </row>
-    <row r="17" spans="1:11" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:11" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A17" s="16">
         <v>3</v>
       </c>
@@ -12395,7 +12402,7 @@
         <v>3500</v>
       </c>
     </row>
-    <row r="18" spans="1:11" ht="26.4" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:11" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A18" s="16"/>
       <c r="B18" s="24" t="s">
         <v>156</v>
@@ -12416,7 +12423,7 @@
         <v>15026.5</v>
       </c>
     </row>
-    <row r="19" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A19" s="16">
         <v>1</v>
       </c>
@@ -12451,7 +12458,7 @@
         <v>96</v>
       </c>
     </row>
-    <row r="20" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A20" s="16">
         <v>2</v>
       </c>
@@ -12483,7 +12490,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="21" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A21" s="16">
         <v>3</v>
       </c>
@@ -12515,7 +12522,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="22" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A22" s="16">
         <v>4</v>
       </c>
@@ -12547,7 +12554,7 @@
         <v>7.5</v>
       </c>
     </row>
-    <row r="23" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A23" s="16">
         <v>5</v>
       </c>
@@ -12579,7 +12586,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="24" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A24" s="16">
         <v>6</v>
       </c>
@@ -12611,7 +12618,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="25" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A25" s="16">
         <v>7</v>
       </c>
@@ -12643,7 +12650,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="26" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A26" s="16">
         <v>8</v>
       </c>
@@ -12675,7 +12682,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="27" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A27" s="16">
         <v>9</v>
       </c>
@@ -12707,7 +12714,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="28" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A28" s="16">
         <v>10</v>
       </c>
@@ -12739,7 +12746,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="29" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A29" s="16">
         <v>11</v>
       </c>
@@ -12771,7 +12778,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="30" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A30" s="16">
         <v>12</v>
       </c>
@@ -12803,7 +12810,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="31" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A31" s="16">
         <v>13</v>
       </c>
@@ -12838,7 +12845,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="32" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A32" s="16">
         <v>14</v>
       </c>
@@ -12873,7 +12880,7 @@
         <v>216</v>
       </c>
     </row>
-    <row r="33" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A33" s="16">
         <v>15</v>
       </c>
@@ -12908,7 +12915,7 @@
         <v>144</v>
       </c>
     </row>
-    <row r="34" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A34" s="16">
         <v>16</v>
       </c>
@@ -12943,7 +12950,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="35" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A35" s="16">
         <v>17</v>
       </c>
@@ -12978,7 +12985,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="36" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A36" s="16">
         <v>18</v>
       </c>
@@ -13010,7 +13017,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="37" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A37" s="16">
         <v>19</v>
       </c>
@@ -13042,7 +13049,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="38" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A38" s="16">
         <v>20</v>
       </c>
@@ -13074,7 +13081,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="39" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A39" s="16">
         <v>21</v>
       </c>
@@ -13106,7 +13113,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="40" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A40" s="16">
         <v>22</v>
       </c>
@@ -13138,7 +13145,7 @@
         <v>10500</v>
       </c>
     </row>
-    <row r="41" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A41" s="16">
         <v>23</v>
       </c>
@@ -13170,7 +13177,7 @@
         <v>1350</v>
       </c>
     </row>
-    <row r="42" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A42" s="16">
         <v>24</v>
       </c>
@@ -13202,7 +13209,7 @@
         <v>350</v>
       </c>
     </row>
-    <row r="43" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A43" s="16">
         <v>25</v>
       </c>
@@ -13234,7 +13241,7 @@
         <v>1500</v>
       </c>
     </row>
-    <row r="44" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="44" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A44" s="16"/>
       <c r="B44" s="18" t="s">
         <v>157</v>
@@ -13255,7 +13262,7 @@
         <v>5205</v>
       </c>
     </row>
-    <row r="45" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="45" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A45" s="16">
         <v>1</v>
       </c>
@@ -13290,7 +13297,7 @@
         <v>3000</v>
       </c>
     </row>
-    <row r="46" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="46" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A46" s="16">
         <v>2</v>
       </c>
@@ -13325,7 +13332,7 @@
         <v>2205</v>
       </c>
     </row>
-    <row r="47" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="47" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A47" s="16"/>
       <c r="B47" s="18" t="s">
         <v>239</v>
@@ -13346,7 +13353,7 @@
         <v>900</v>
       </c>
     </row>
-    <row r="48" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="48" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A48" s="16">
         <v>1</v>
       </c>
@@ -13381,7 +13388,7 @@
         <v>150</v>
       </c>
     </row>
-    <row r="49" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="49" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A49" s="16">
         <v>2</v>
       </c>
@@ -13416,7 +13423,7 @@
         <v>150</v>
       </c>
     </row>
-    <row r="50" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="50" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A50" s="16">
         <v>4</v>
       </c>
@@ -13451,7 +13458,7 @@
         <v>150</v>
       </c>
     </row>
-    <row r="51" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="51" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A51" s="16">
         <v>5</v>
       </c>
@@ -13486,7 +13493,7 @@
         <v>150</v>
       </c>
     </row>
-    <row r="52" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="52" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A52" s="16">
         <v>6</v>
       </c>
@@ -13521,7 +13528,7 @@
         <v>150</v>
       </c>
     </row>
-    <row r="53" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="53" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A53" s="16">
         <v>7</v>
       </c>
@@ -13556,7 +13563,7 @@
         <v>150</v>
       </c>
     </row>
-    <row r="54" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="54" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A54" s="31"/>
       <c r="B54" s="35" t="s">
         <v>204</v>
@@ -13589,14 +13596,14 @@
         <v>5000</v>
       </c>
     </row>
-    <row r="55" spans="1:11" ht="23.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B55" s="115" t="s">
+    <row r="55" spans="1:11" ht="23.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B55" s="121" t="s">
         <v>25</v>
       </c>
-      <c r="C55" s="116"/>
-      <c r="D55" s="116"/>
-      <c r="E55" s="116"/>
-      <c r="F55" s="117"/>
+      <c r="C55" s="122"/>
+      <c r="D55" s="122"/>
+      <c r="E55" s="122"/>
+      <c r="F55" s="123"/>
       <c r="G55" s="6">
         <f>+G3+G12+G14+G18+G44+G47+G54</f>
         <v>101031.5</v>
@@ -13618,13 +13625,13 @@
         <v>101031.5</v>
       </c>
     </row>
-    <row r="56" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="56" spans="1:11" x14ac:dyDescent="0.2">
       <c r="K56" s="30">
         <f>SUM(H55:J55)</f>
         <v>101031.5</v>
       </c>
     </row>
-    <row r="59" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="59" spans="1:11" x14ac:dyDescent="0.2">
       <c r="G59" s="30"/>
     </row>
   </sheetData>

</xml_diff>